<commit_message>
finish the header interactive mode
</commit_message>
<xml_diff>
--- a/invoice_gen/TEMPLATE/OJY.xlsx
+++ b/invoice_gen/TEMPLATE/OJY.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Contract" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Packing list" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Invoice" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Contract" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Packing list" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Invoice" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Contract'!$A$1:$F$37</definedName>
@@ -823,7 +823,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor>
     <from>
       <col>7</col>
@@ -843,7 +843,7 @@
         <cNvGrpSpPr/>
       </nvGrpSpPr>
       <grpSpPr>
-        <a:xfrm rot="0">
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0">
           <a:off x="10344150" y="11494770"/>
           <a:ext cx="3075940" cy="1517650"/>
           <a:chOff x="7095490" y="13465334"/>
@@ -854,24 +854,24 @@
         <nvPicPr>
           <cNvPr id="4" name="图片 2" descr="微信图片_20231124163945"/>
           <cNvPicPr>
-            <a:picLocks noChangeAspect="1"/>
+            <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
           </cNvPicPr>
         </nvPicPr>
         <blipFill>
-          <a:blip r:embed="rId1"/>
-          <a:stretch>
+          <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:fillRect/>
           </a:stretch>
         </blipFill>
         <spPr>
-          <a:xfrm>
+          <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:off x="9526289" y="14283149"/>
             <a:ext cx="2179637" cy="1332388"/>
           </a:xfrm>
-          <a:prstGeom prst="rect">
+          <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
             <avLst/>
           </a:prstGeom>
-          <a:ln>
+          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:prstDash val="solid"/>
           </a:ln>
         </spPr>
@@ -883,7 +883,7 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor>
     <from>
       <col>11</col>
@@ -903,7 +903,7 @@
         <cNvGrpSpPr/>
       </nvGrpSpPr>
       <grpSpPr>
-        <a:xfrm rot="0">
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0">
           <a:off x="13679805" y="9572625"/>
           <a:ext cx="3124200" cy="1207770"/>
           <a:chOff x="7095490" y="13465334"/>
@@ -914,24 +914,24 @@
         <nvPicPr>
           <cNvPr id="4" name="图片 2" descr="微信图片_20231124163945"/>
           <cNvPicPr>
-            <a:picLocks noChangeAspect="1"/>
+            <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
           </cNvPicPr>
         </nvPicPr>
         <blipFill>
-          <a:blip r:embed="rId1"/>
-          <a:stretch>
+          <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:fillRect/>
           </a:stretch>
         </blipFill>
         <spPr>
-          <a:xfrm>
+          <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:off x="9526289" y="14283149"/>
             <a:ext cx="2179637" cy="1332388"/>
           </a:xfrm>
-          <a:prstGeom prst="rect">
+          <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
             <avLst/>
           </a:prstGeom>
-          <a:ln>
+          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:prstDash val="solid"/>
           </a:ln>
         </spPr>
@@ -943,7 +943,7 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <twoCellAnchor>
     <from>
       <col>7</col>
@@ -963,7 +963,7 @@
         <cNvGrpSpPr/>
       </nvGrpSpPr>
       <grpSpPr>
-        <a:xfrm rot="0">
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" rot="0">
           <a:off x="11498313" y="8389486"/>
           <a:ext cx="3138269" cy="1459984"/>
           <a:chOff x="7095490" y="13465334"/>
@@ -974,24 +974,24 @@
         <nvPicPr>
           <cNvPr id="4" name="图片 2" descr="微信图片_20231124163945"/>
           <cNvPicPr>
-            <a:picLocks noChangeAspect="1"/>
+            <a:picLocks xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" noChangeAspect="1"/>
           </cNvPicPr>
         </nvPicPr>
         <blipFill>
-          <a:blip r:embed="rId1"/>
-          <a:stretch>
+          <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:fillRect/>
           </a:stretch>
         </blipFill>
         <spPr>
-          <a:xfrm>
+          <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:off x="9526289" y="14283149"/>
             <a:ext cx="2179637" cy="1332388"/>
           </a:xfrm>
-          <a:prstGeom prst="rect">
+          <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
             <avLst/>
           </a:prstGeom>
-          <a:ln>
+          <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
             <a:prstDash val="solid"/>
           </a:ln>
         </spPr>
@@ -1484,305 +1484,181 @@
         </is>
       </c>
     </row>
-    <row r="20" ht="28.95" customHeight="1" s="107">
-      <c r="A20" s="67" t="inlineStr">
-        <is>
-          <t>P.O Nº</t>
-        </is>
-      </c>
-      <c r="B20" s="67" t="inlineStr">
-        <is>
-          <t>Name of Cormodity
-Tên và miêu tả</t>
-        </is>
-      </c>
-      <c r="C20" s="67" t="inlineStr">
-        <is>
-          <t>Description
-Tả hàng hóa</t>
-        </is>
-      </c>
-      <c r="D20" s="67" t="inlineStr">
-        <is>
-          <t>Quantity(SF)
-Số lượng(SF)</t>
-        </is>
-      </c>
-      <c r="E20" s="67" t="inlineStr">
-        <is>
-          <t>Unit Price(USD)
-Đơn giá</t>
-        </is>
-      </c>
-      <c r="F20" s="67" t="inlineStr">
-        <is>
-          <t>Total value(USD)
-Trị giá</t>
-        </is>
-      </c>
-    </row>
-    <row r="21" ht="21" customHeight="1" s="107">
-      <c r="A21" s="68" t="inlineStr">
-        <is>
-          <t>YNGYML25005</t>
-        </is>
-      </c>
-      <c r="B21" s="68" t="inlineStr">
-        <is>
-          <t>Nick Dove</t>
-        </is>
-      </c>
-      <c r="C21" s="90" t="inlineStr">
-        <is>
-          <t>COW LEATHER
-DA BÒ THUỘC</t>
-        </is>
-      </c>
-      <c r="D21" s="69" t="n">
-        <v>149828</v>
-      </c>
-      <c r="E21" s="70">
-        <f>F21/D21</f>
-        <v/>
-      </c>
-      <c r="F21" s="69" t="n">
-        <v>154180.0402727273</v>
-      </c>
-    </row>
+    <row r="20" ht="28.95" customHeight="1" s="107"/>
+    <row r="21" ht="21" customHeight="1" s="107"/>
     <row r="22" ht="21" customHeight="1" s="107">
-      <c r="A22" s="68" t="inlineStr">
-        <is>
-          <t>YNGYML25005</t>
-        </is>
-      </c>
-      <c r="B22" s="68" t="inlineStr">
-        <is>
-          <t>M1243</t>
-        </is>
-      </c>
-      <c r="C22" s="91" t="n"/>
-      <c r="D22" s="69" t="n">
-        <v>41895.9</v>
-      </c>
-      <c r="E22" s="70">
-        <f>F22/D22</f>
-        <v/>
-      </c>
-      <c r="F22" s="69" t="n">
-        <v>42156.52154545454</v>
-      </c>
-    </row>
-    <row r="23" ht="21" customFormat="1" customHeight="1" s="96">
-      <c r="A23" s="68" t="inlineStr">
-        <is>
-          <t>OJY_0015</t>
-        </is>
-      </c>
-      <c r="B23" s="68" t="inlineStr">
-        <is>
-          <t>Nick Dove</t>
-        </is>
-      </c>
-      <c r="C23" s="92" t="n"/>
-      <c r="D23" s="69" t="n">
-        <v>64377.8</v>
-      </c>
-      <c r="E23" s="70">
-        <f>F23/D23</f>
-        <v/>
-      </c>
-      <c r="F23" s="69" t="n">
-        <v>66952.70818181818</v>
+      <c r="A22" s="93" t="n"/>
+      <c r="B22" s="93" t="n"/>
+      <c r="C22" s="93" t="n"/>
+      <c r="D22" s="93" t="n"/>
+      <c r="E22" s="93" t="n"/>
+      <c r="F22" s="93" t="n"/>
+    </row>
+    <row r="23" ht="29.1" customFormat="1" customHeight="1" s="96">
+      <c r="A23" s="93" t="inlineStr">
+        <is>
+          <t>Người bán, người mua và người thụ hưởng đã thống nhất đồng ý các giao dịch sau theo các điều khoản và điều kiện được quy định dưới đây:</t>
+        </is>
       </c>
     </row>
     <row r="24" ht="28.95" customFormat="1" customHeight="1" s="96">
-      <c r="A24" s="88" t="inlineStr">
-        <is>
-          <t>TOTAL AMOUNT(Tổng trị giá):</t>
-        </is>
-      </c>
-      <c r="B24" s="89" t="n"/>
-      <c r="C24" s="88" t="n"/>
-      <c r="D24" s="72">
-        <f>SUM(D21:D23)</f>
-        <v/>
-      </c>
-      <c r="E24" s="88" t="n"/>
-      <c r="F24" s="72">
-        <f>SUM(F21:F23)</f>
-        <v/>
-      </c>
+      <c r="A24" s="51" t="inlineStr">
+        <is>
+          <t>FCA:</t>
+        </is>
+      </c>
+      <c r="B24" s="52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BAVET,SVAYRIENG </t>
+        </is>
+      </c>
+      <c r="C24" s="52" t="n"/>
+      <c r="D24" s="44" t="n"/>
+      <c r="E24" s="44" t="n"/>
+      <c r="F24" s="55" t="n"/>
     </row>
     <row r="25" ht="29.1" customFormat="1" customHeight="1" s="96">
-      <c r="A25" s="93" t="n"/>
-      <c r="B25" s="93" t="n"/>
-      <c r="C25" s="93" t="n"/>
-      <c r="D25" s="93" t="n"/>
-      <c r="E25" s="93" t="n"/>
-      <c r="F25" s="93" t="n"/>
+      <c r="A25" s="44" t="inlineStr">
+        <is>
+          <t>Term of Payment: 100% TT after shipment(Điều kiện thanh toán: 100% T/T, thời hạn thanh toán sau khi giao hàng)</t>
+        </is>
+      </c>
+      <c r="B25" s="44" t="n"/>
+      <c r="C25" s="44" t="n"/>
+      <c r="D25" s="44" t="n"/>
+      <c r="E25" s="44" t="n"/>
+      <c r="F25" s="44" t="n"/>
     </row>
     <row r="26" ht="29.1" customFormat="1" customHeight="1" s="96">
-      <c r="A26" s="93" t="inlineStr">
-        <is>
-          <t>Người bán, người mua và người thụ hưởng đã thống nhất đồng ý các giao dịch sau theo các điều khoản và điều kiện được quy định dưới đây:</t>
-        </is>
-      </c>
+      <c r="A26" s="44" t="inlineStr">
+        <is>
+          <t>Transaction method: FCA(USD)  (Phương thức giao hàng: FCA(USD))</t>
+        </is>
+      </c>
+      <c r="B26" s="44" t="n"/>
+      <c r="C26" s="44" t="n"/>
+      <c r="D26" s="44" t="n"/>
+      <c r="E26" s="44" t="n"/>
+      <c r="F26" s="44" t="n"/>
     </row>
     <row r="27" ht="45.9" customFormat="1" customHeight="1" s="96">
-      <c r="A27" s="51" t="inlineStr">
-        <is>
-          <t>FCA:</t>
-        </is>
-      </c>
-      <c r="B27" s="52" t="inlineStr">
-        <is>
-          <t xml:space="preserve">BAVET,SVAYRIENG </t>
-        </is>
-      </c>
-      <c r="C27" s="52" t="n"/>
-      <c r="D27" s="44" t="n"/>
+      <c r="A27" s="44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beneficiary bank information(Thông tin ngân hàng thụ hưởng): </t>
+        </is>
+      </c>
+      <c r="B27" s="44" t="n"/>
+      <c r="C27" s="44" t="n"/>
+      <c r="D27" s="44" t="inlineStr">
+        <is>
+          <t>CALIFOR UPHOLSTERY MATERIALS CO.,LTD.</t>
+        </is>
+      </c>
       <c r="E27" s="44" t="n"/>
-      <c r="F27" s="55" t="n"/>
-    </row>
-    <row r="28" ht="41.1" customFormat="1" customHeight="1" s="96">
+      <c r="F27" s="44" t="n"/>
+    </row>
+    <row r="28" ht="45.9" customFormat="1" customHeight="1" s="96">
       <c r="A28" s="44" t="inlineStr">
         <is>
-          <t>Term of Payment: 100% TT after shipment(Điều kiện thanh toán: 100% T/T, thời hạn thanh toán sau khi giao hàng)</t>
+          <t xml:space="preserve">Beneficiary Bank' s Name(Tên ngân hàng thụ hưởng): </t>
         </is>
       </c>
       <c r="B28" s="44" t="n"/>
       <c r="C28" s="44" t="n"/>
-      <c r="D28" s="44" t="n"/>
-      <c r="E28" s="44" t="n"/>
-      <c r="F28" s="44" t="n"/>
-    </row>
-    <row r="29" ht="29.1" customFormat="1" customHeight="1" s="96">
+      <c r="D28" s="93" t="inlineStr">
+        <is>
+          <t>BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH
+ /BANK OF CHINA PHNOM PENH BRANCH</t>
+        </is>
+      </c>
+    </row>
+    <row r="29" ht="41.1" customFormat="1" customHeight="1" s="96">
       <c r="A29" s="44" t="inlineStr">
         <is>
-          <t>Transaction method: FCA(USD)  (Phương thức giao hàng: FCA(USD))</t>
+          <t xml:space="preserve">Bank Address( địa chỉ ngân hàng):  </t>
         </is>
       </c>
       <c r="B29" s="44" t="n"/>
       <c r="C29" s="44" t="n"/>
-      <c r="D29" s="44" t="n"/>
-      <c r="E29" s="44" t="n"/>
-      <c r="F29" s="44" t="n"/>
+      <c r="D29" s="93" t="inlineStr">
+        <is>
+          <t>1st AND 2nd FLOOR,CANADIA TOWER,No.315 ANDDUONG ST.
+PHNOM PEMH,CAMBODIA.</t>
+        </is>
+      </c>
     </row>
     <row r="30" ht="29.1" customFormat="1" customHeight="1" s="96">
       <c r="A30" s="44" t="inlineStr">
         <is>
-          <t xml:space="preserve">Beneficiary bank information(Thông tin ngân hàng thụ hưởng): </t>
+          <t>Bank account(số tài khoản) :</t>
         </is>
       </c>
       <c r="B30" s="44" t="n"/>
       <c r="C30" s="44" t="n"/>
-      <c r="D30" s="44" t="inlineStr">
-        <is>
-          <t>CALIFOR UPHOLSTERY MATERIALS CO.,LTD.</t>
-        </is>
-      </c>
-      <c r="E30" s="44" t="n"/>
-      <c r="F30" s="44" t="n"/>
+      <c r="D30" s="102" t="inlineStr">
+        <is>
+          <t>100001100764430</t>
+        </is>
+      </c>
     </row>
     <row r="31" ht="45.9" customFormat="1" customHeight="1" s="96">
       <c r="A31" s="44" t="inlineStr">
         <is>
-          <t xml:space="preserve">Beneficiary Bank' s Name(Tên ngân hàng thụ hưởng): </t>
+          <t>SWIFT CODE( mã swift)  ：</t>
         </is>
       </c>
       <c r="B31" s="44" t="n"/>
       <c r="C31" s="44" t="n"/>
-      <c r="D31" s="93" t="inlineStr">
-        <is>
-          <t>BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH
- /BANK OF CHINA PHNOM PENH BRANCH</t>
-        </is>
-      </c>
+      <c r="D31" s="44" t="inlineStr">
+        <is>
+          <t>BKCHKHPPXXX</t>
+        </is>
+      </c>
+      <c r="E31" s="44" t="n"/>
+      <c r="F31" s="44" t="n"/>
     </row>
     <row r="32" ht="41.1" customFormat="1" customHeight="1" s="94">
-      <c r="A32" s="44" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Bank Address( địa chỉ ngân hàng):  </t>
-        </is>
-      </c>
+      <c r="A32" s="44" t="n"/>
       <c r="B32" s="44" t="n"/>
       <c r="C32" s="44" t="n"/>
-      <c r="D32" s="93" t="inlineStr">
-        <is>
-          <t>1st AND 2nd FLOOR,CANADIA TOWER,No.315 ANDDUONG ST.
-PHNOM PEMH,CAMBODIA.</t>
-        </is>
-      </c>
+      <c r="D32" s="44" t="n"/>
+      <c r="E32" s="44" t="n"/>
+      <c r="F32" s="44" t="n"/>
+      <c r="G32" s="53" t="n"/>
     </row>
     <row r="33" ht="29.1" customFormat="1" customHeight="1" s="94">
-      <c r="A33" s="44" t="inlineStr">
-        <is>
-          <t>Bank account(số tài khoản) :</t>
-        </is>
-      </c>
-      <c r="B33" s="44" t="n"/>
-      <c r="C33" s="44" t="n"/>
-      <c r="D33" s="102" t="inlineStr">
-        <is>
-          <t>100001100764430</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="44" t="inlineStr">
-        <is>
-          <t>SWIFT CODE( mã swift)  ：</t>
-        </is>
-      </c>
-      <c r="B34" s="44" t="n"/>
-      <c r="C34" s="44" t="n"/>
-      <c r="D34" s="44" t="inlineStr">
-        <is>
-          <t>BKCHKHPPXXX</t>
-        </is>
-      </c>
-      <c r="E34" s="44" t="n"/>
-      <c r="F34" s="44" t="n"/>
-    </row>
-    <row r="35" ht="19.2" customHeight="1" s="107">
-      <c r="A35" s="44" t="n"/>
-      <c r="B35" s="44" t="n"/>
-      <c r="C35" s="44" t="n"/>
-      <c r="D35" s="44" t="n"/>
-      <c r="E35" s="44" t="n"/>
-      <c r="F35" s="44" t="n"/>
-      <c r="G35" s="53" t="n"/>
-    </row>
-    <row r="36">
-      <c r="A36" s="46" t="inlineStr">
+      <c r="A33" s="46" t="inlineStr">
         <is>
           <t>The Buyer(bên mua):</t>
         </is>
       </c>
-      <c r="B36" s="46" t="n"/>
-      <c r="C36" s="46" t="n"/>
-      <c r="D36" s="46" t="n"/>
-      <c r="E36" s="44" t="inlineStr">
+      <c r="B33" s="46" t="n"/>
+      <c r="C33" s="46" t="n"/>
+      <c r="D33" s="46" t="n"/>
+      <c r="E33" s="44" t="inlineStr">
         <is>
           <t>The Seller(bên bán):</t>
         </is>
       </c>
-      <c r="F36" s="46" t="n"/>
-    </row>
-    <row r="37" ht="57" customHeight="1" s="107">
-      <c r="A37" s="100" t="inlineStr">
+      <c r="F33" s="46" t="n"/>
+    </row>
+    <row r="34" ht="57" customHeight="1" s="107">
+      <c r="A34" s="100" t="inlineStr">
         <is>
           <t>OUCANYON FURNITURE ( VIETNAM) CO.,LTD.</t>
         </is>
       </c>
-      <c r="C37" s="100" t="n"/>
-      <c r="D37" s="93" t="n"/>
-      <c r="E37" s="100" t="inlineStr">
+      <c r="C34" s="100" t="n"/>
+      <c r="D34" s="93" t="n"/>
+      <c r="E34" s="100" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO.,LTD.</t>
         </is>
       </c>
     </row>
+    <row r="35" ht="19.2" customHeight="1" s="107"/>
+    <row r="36"/>
+    <row r="37" ht="57" customHeight="1" s="107"/>
     <row r="38"/>
     <row r="39"/>
     <row r="40"/>
@@ -1947,28 +1823,26 @@
     <row r="199"/>
     <row r="200"/>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C21:C23"/>
-    <mergeCell ref="D32:F32"/>
+  <mergeCells count="19">
     <mergeCell ref="A18:F18"/>
-    <mergeCell ref="A26:F26"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="B12:F12"/>
+    <mergeCell ref="D28:F28"/>
     <mergeCell ref="B11:F11"/>
-    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A23:F23"/>
     <mergeCell ref="B14:F14"/>
-    <mergeCell ref="D33:F33"/>
+    <mergeCell ref="D30:F30"/>
     <mergeCell ref="B13:F13"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="D29:F29"/>
     <mergeCell ref="A19:F19"/>
     <mergeCell ref="B10:F10"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="B9:F9"/>
-    <mergeCell ref="D31:F31"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="B5:F5"/>
-    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A34:B34"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.1" right="0.1" top="0.75" bottom="0.75" header="0.5" footer="0.5"/>

</xml_diff>